<commit_message>
Even better unit tests now... FakeDeque now also implements GetReverseView method.
</commit_message>
<xml_diff>
--- a/Tabulka_funkci.xlsx
+++ b/Tabulka_funkci.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sony\Desktop\programovani - projekty\C#\PokrNET_I\Deque_2_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:0_{6E8AB893-BB9B-4B9C-8BBA-80A8909F6490}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A1896A6-1AC4-4549-AA20-D4634E42F130}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1185" yWindow="1125" windowWidth="10800" windowHeight="8985" xr2:uid="{E8082D59-5A8F-4B45-9A2C-CE2EBB755BD9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{E8082D59-5A8F-4B45-9A2C-CE2EBB755BD9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -449,7 +449,7 @@
   <dimension ref="A1:AH16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="AG9" sqref="AG9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -458,9 +458,13 @@
     <col min="2" max="3" width="3.42578125" customWidth="1"/>
     <col min="4" max="8" width="3.42578125" style="1" customWidth="1"/>
     <col min="9" max="13" width="3.42578125" customWidth="1"/>
-    <col min="14" max="20" width="3.42578125" style="1" customWidth="1"/>
+    <col min="14" max="15" width="3.42578125" style="3" customWidth="1"/>
+    <col min="16" max="16" width="3.42578125" style="1" customWidth="1"/>
+    <col min="17" max="18" width="3.42578125" style="3" customWidth="1"/>
+    <col min="19" max="20" width="3.42578125" style="1" customWidth="1"/>
     <col min="21" max="23" width="3.42578125" customWidth="1"/>
-    <col min="24" max="27" width="3.42578125" style="1" customWidth="1"/>
+    <col min="24" max="26" width="3.42578125" style="1" customWidth="1"/>
+    <col min="27" max="27" width="3.42578125" style="3" customWidth="1"/>
     <col min="28" max="34" width="3.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -501,19 +505,19 @@
       <c r="M1">
         <v>12</v>
       </c>
-      <c r="N1" s="1">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1">
+      <c r="N1" s="3">
+        <v>13</v>
+      </c>
+      <c r="O1" s="3">
         <v>14</v>
       </c>
       <c r="P1" s="1">
         <v>15</v>
       </c>
-      <c r="Q1" s="1">
+      <c r="Q1" s="3">
         <v>16</v>
       </c>
-      <c r="R1" s="1">
+      <c r="R1" s="3">
         <v>17</v>
       </c>
       <c r="S1" s="1">
@@ -540,7 +544,7 @@
       <c r="Z1" s="1">
         <v>25</v>
       </c>
-      <c r="AA1" s="1">
+      <c r="AA1" s="3">
         <v>26</v>
       </c>
       <c r="AB1">
@@ -605,19 +609,19 @@
       <c r="M2" t="s">
         <v>13</v>
       </c>
-      <c r="N2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O2" s="1" t="s">
+      <c r="N2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="O2" s="3" t="s">
         <v>13</v>
       </c>
       <c r="P2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="Q2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="R2" s="1" t="s">
+      <c r="Q2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="R2" s="3" t="s">
         <v>13</v>
       </c>
       <c r="S2" s="1" t="s">
@@ -644,7 +648,7 @@
       <c r="Z2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="AA2" s="1" t="s">
+      <c r="AA2" s="3" t="s">
         <v>13</v>
       </c>
       <c r="AB2" t="s">
@@ -688,19 +692,19 @@
       <c r="M3" t="s">
         <v>13</v>
       </c>
-      <c r="N3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O3" s="1" t="s">
+      <c r="N3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="O3" s="3" t="s">
         <v>13</v>
       </c>
       <c r="P3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="Q3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="R3" s="1" t="s">
+      <c r="Q3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="R3" s="3" t="s">
         <v>13</v>
       </c>
       <c r="S3" s="1" t="s">
@@ -765,19 +769,19 @@
       <c r="M4" t="s">
         <v>13</v>
       </c>
-      <c r="N4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O4" s="1" t="s">
+      <c r="N4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="O4" s="3" t="s">
         <v>13</v>
       </c>
       <c r="P4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="Q4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="R4" s="1" t="s">
+      <c r="Q4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="R4" s="3" t="s">
         <v>13</v>
       </c>
       <c r="S4" s="1" t="s">
@@ -804,7 +808,7 @@
       <c r="Z4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="AA4" s="1" t="s">
+      <c r="AA4" s="3" t="s">
         <v>13</v>
       </c>
       <c r="AB4" t="s">
@@ -848,19 +852,19 @@
       <c r="M5" t="s">
         <v>13</v>
       </c>
-      <c r="N5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O5" s="1" t="s">
+      <c r="N5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="O5" s="3" t="s">
         <v>13</v>
       </c>
       <c r="P5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="Q5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="R5" s="1" t="s">
+      <c r="Q5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="R5" s="3" t="s">
         <v>13</v>
       </c>
       <c r="S5" s="1" t="s">
@@ -887,7 +891,7 @@
       <c r="Z5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="AA5" s="1" t="s">
+      <c r="AA5" s="3" t="s">
         <v>13</v>
       </c>
       <c r="AB5" t="s">
@@ -928,19 +932,19 @@
       <c r="M6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="N6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O6" s="1" t="s">
+      <c r="N6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="O6" s="3" t="s">
         <v>13</v>
       </c>
       <c r="P6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="Q6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="R6" s="1" t="s">
+      <c r="Q6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="R6" s="3" t="s">
         <v>13</v>
       </c>
       <c r="S6" s="1" t="s">
@@ -961,7 +965,7 @@
       <c r="Z6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="AA6" s="1" t="s">
+      <c r="AA6" s="3" t="s">
         <v>13</v>
       </c>
     </row>
@@ -981,7 +985,7 @@
       <c r="X7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="AA7" s="1" t="s">
+      <c r="AA7" s="3" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1016,16 +1020,16 @@
       <c r="M8" t="s">
         <v>13</v>
       </c>
-      <c r="N8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="R8" s="1" t="s">
+      <c r="N8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="O8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="R8" s="3" t="s">
         <v>13</v>
       </c>
       <c r="U8" t="s">
@@ -1057,16 +1061,16 @@
       <c r="M9" t="s">
         <v>13</v>
       </c>
-      <c r="N9" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O9" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q9" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="R9" s="1" t="s">
+      <c r="N9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="O9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="R9" s="3" t="s">
         <v>13</v>
       </c>
       <c r="S9" s="1" t="s">
@@ -1101,7 +1105,7 @@
       <c r="Z10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="AA10" s="1" t="s">
+      <c r="AA10" s="3" t="s">
         <v>13</v>
       </c>
       <c r="AB10" t="s">
@@ -1127,16 +1131,16 @@
       <c r="M11" t="s">
         <v>13</v>
       </c>
-      <c r="N11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="R11" s="1" t="s">
+      <c r="N11" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="O11" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q11" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="R11" s="3" t="s">
         <v>13</v>
       </c>
       <c r="U11" t="s">
@@ -1157,7 +1161,7 @@
       <c r="Z11" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="AA11" s="1" t="s">
+      <c r="AA11" s="3" t="s">
         <v>13</v>
       </c>
       <c r="AB11" t="s">
@@ -1165,19 +1169,19 @@
       </c>
     </row>
     <row r="12" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="N12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="R12" s="1" t="s">
+      <c r="N12" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="O12" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q12" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="R12" s="3" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1188,10 +1192,10 @@
       <c r="P13" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="Q13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="R13" s="1" t="s">
+      <c r="Q13" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="R13" s="3" t="s">
         <v>13</v>
       </c>
       <c r="T13" s="1" t="s">
@@ -1222,7 +1226,7 @@
       <c r="X15" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="AA15" s="1" t="s">
+      <c r="AA15" s="3" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
We can peek in deque now. Adding in deque now works better. Disposed enumerator no longer works. A few unitTests were added.
</commit_message>
<xml_diff>
--- a/Tabulka_funkci.xlsx
+++ b/Tabulka_funkci.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sony\Desktop\programovani - projekty\C#\PokrNET_I\Deque_2_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A1896A6-1AC4-4549-AA20-D4634E42F130}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6475E5E-9A69-4CB6-A09D-8340E44CBCB3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{E8082D59-5A8F-4B45-9A2C-CE2EBB755BD9}"/>
   </bookViews>
@@ -449,18 +449,16 @@
   <dimension ref="A1:AH16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AG9" sqref="AG9"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="3.42578125" customWidth="1"/>
-    <col min="4" max="8" width="3.42578125" style="1" customWidth="1"/>
+    <col min="4" max="8" width="3.42578125" style="3" customWidth="1"/>
     <col min="9" max="13" width="3.42578125" customWidth="1"/>
-    <col min="14" max="15" width="3.42578125" style="3" customWidth="1"/>
-    <col min="16" max="16" width="3.42578125" style="1" customWidth="1"/>
-    <col min="17" max="18" width="3.42578125" style="3" customWidth="1"/>
+    <col min="14" max="18" width="3.42578125" style="3" customWidth="1"/>
     <col min="19" max="20" width="3.42578125" style="1" customWidth="1"/>
     <col min="21" max="23" width="3.42578125" customWidth="1"/>
     <col min="24" max="26" width="3.42578125" style="1" customWidth="1"/>
@@ -475,19 +473,19 @@
       <c r="C1">
         <v>2</v>
       </c>
-      <c r="D1" s="1">
+      <c r="D1" s="3">
         <v>3</v>
       </c>
-      <c r="E1" s="1">
+      <c r="E1" s="3">
         <v>4</v>
       </c>
-      <c r="F1" s="1">
+      <c r="F1" s="3">
         <v>5</v>
       </c>
-      <c r="G1" s="1">
+      <c r="G1" s="3">
         <v>6</v>
       </c>
-      <c r="H1" s="1">
+      <c r="H1" s="3">
         <v>7</v>
       </c>
       <c r="I1">
@@ -511,7 +509,7 @@
       <c r="O1" s="3">
         <v>14</v>
       </c>
-      <c r="P1" s="1">
+      <c r="P1" s="3">
         <v>15</v>
       </c>
       <c r="Q1" s="3">
@@ -579,19 +577,19 @@
       <c r="C2" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" s="1" t="s">
+      <c r="D2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>13</v>
       </c>
       <c r="I2" t="s">
@@ -615,7 +613,7 @@
       <c r="O2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="P2" s="3" t="s">
         <v>13</v>
       </c>
       <c r="Q2" s="3" t="s">
@@ -662,19 +660,19 @@
       <c r="B3" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" s="1" t="s">
+      <c r="D3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="3" t="s">
         <v>13</v>
       </c>
       <c r="I3" t="s">
@@ -698,7 +696,7 @@
       <c r="O3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="P3" s="1" t="s">
+      <c r="P3" s="3" t="s">
         <v>13</v>
       </c>
       <c r="Q3" s="3" t="s">
@@ -739,19 +737,19 @@
       <c r="C4" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" s="1" t="s">
+      <c r="D4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="3" t="s">
         <v>13</v>
       </c>
       <c r="I4" t="s">
@@ -775,7 +773,7 @@
       <c r="O4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="P4" s="1" t="s">
+      <c r="P4" s="3" t="s">
         <v>13</v>
       </c>
       <c r="Q4" s="3" t="s">
@@ -822,19 +820,19 @@
       <c r="C5" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H5" s="1" t="s">
+      <c r="D5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" s="3" t="s">
         <v>13</v>
       </c>
       <c r="I5" t="s">
@@ -858,7 +856,7 @@
       <c r="O5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="P5" s="1" t="s">
+      <c r="P5" s="3" t="s">
         <v>13</v>
       </c>
       <c r="Q5" s="3" t="s">
@@ -902,19 +900,19 @@
       <c r="A6" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H6" s="1" t="s">
+      <c r="D6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" s="3" t="s">
         <v>13</v>
       </c>
       <c r="I6" s="3" t="s">
@@ -938,7 +936,7 @@
       <c r="O6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="P6" s="1" t="s">
+      <c r="P6" s="3" t="s">
         <v>13</v>
       </c>
       <c r="Q6" s="3" t="s">
@@ -973,13 +971,13 @@
       <c r="A7" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="P7" s="1" t="s">
+      <c r="D7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="P7" s="3" t="s">
         <v>13</v>
       </c>
       <c r="X7" s="1" t="s">
@@ -990,19 +988,19 @@
       </c>
     </row>
     <row r="8" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H8" s="1" t="s">
+      <c r="E8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" s="3" t="s">
         <v>13</v>
       </c>
       <c r="I8" t="s">
@@ -1040,10 +1038,10 @@
       <c r="A9" t="s">
         <v>6</v>
       </c>
-      <c r="G9" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H9" s="1" t="s">
+      <c r="G9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9" s="3" t="s">
         <v>13</v>
       </c>
       <c r="I9" t="s">
@@ -1084,7 +1082,7 @@
       <c r="A10" t="s">
         <v>7</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="G10" s="3" t="s">
         <v>13</v>
       </c>
       <c r="U10" t="s">
@@ -1189,7 +1187,7 @@
       <c r="A13" t="s">
         <v>9</v>
       </c>
-      <c r="P13" s="1" t="s">
+      <c r="P13" s="3" t="s">
         <v>13</v>
       </c>
       <c r="Q13" s="3" t="s">

</xml_diff>

<commit_message>
Insert and InvertedView.IndexOf now works better.
Whole new part of null-unitTests added,
</commit_message>
<xml_diff>
--- a/Tabulka_funkci.xlsx
+++ b/Tabulka_funkci.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sony\Desktop\programovani - projekty\C#\PokrNET_I\Deque_2_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6475E5E-9A69-4CB6-A09D-8340E44CBCB3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30E48A8A-BE89-4768-9902-D920C79DCCFE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{E8082D59-5A8F-4B45-9A2C-CE2EBB755BD9}"/>
   </bookViews>
@@ -449,7 +449,7 @@
   <dimension ref="A1:AH16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="T9" sqref="T9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -461,8 +461,7 @@
     <col min="14" max="18" width="3.42578125" style="3" customWidth="1"/>
     <col min="19" max="20" width="3.42578125" style="1" customWidth="1"/>
     <col min="21" max="23" width="3.42578125" customWidth="1"/>
-    <col min="24" max="26" width="3.42578125" style="1" customWidth="1"/>
-    <col min="27" max="27" width="3.42578125" style="3" customWidth="1"/>
+    <col min="24" max="27" width="3.42578125" style="3" customWidth="1"/>
     <col min="28" max="34" width="3.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -533,13 +532,13 @@
       <c r="W1">
         <v>22</v>
       </c>
-      <c r="X1" s="1">
+      <c r="X1" s="3">
         <v>23</v>
       </c>
-      <c r="Y1" s="1">
+      <c r="Y1" s="3">
         <v>24</v>
       </c>
-      <c r="Z1" s="1">
+      <c r="Z1" s="3">
         <v>25</v>
       </c>
       <c r="AA1" s="3">
@@ -637,13 +636,13 @@
       <c r="W2" t="s">
         <v>13</v>
       </c>
-      <c r="X2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z2" s="1" t="s">
+      <c r="X2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z2" s="3" t="s">
         <v>13</v>
       </c>
       <c r="AA2" s="3" t="s">
@@ -720,13 +719,13 @@
       <c r="W3" t="s">
         <v>13</v>
       </c>
-      <c r="X3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z3" s="1" t="s">
+      <c r="X3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z3" s="3" t="s">
         <v>13</v>
       </c>
     </row>
@@ -797,13 +796,13 @@
       <c r="W4" t="s">
         <v>13</v>
       </c>
-      <c r="X4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z4" s="1" t="s">
+      <c r="X4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z4" s="3" t="s">
         <v>13</v>
       </c>
       <c r="AA4" s="3" t="s">
@@ -880,13 +879,13 @@
       <c r="W5" t="s">
         <v>13</v>
       </c>
-      <c r="X5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z5" s="1" t="s">
+      <c r="X5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z5" s="3" t="s">
         <v>13</v>
       </c>
       <c r="AA5" s="3" t="s">
@@ -954,13 +953,13 @@
       <c r="U6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="X6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z6" s="1" t="s">
+      <c r="X6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z6" s="3" t="s">
         <v>13</v>
       </c>
       <c r="AA6" s="3" t="s">
@@ -968,7 +967,7 @@
       </c>
     </row>
     <row r="7" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D7" s="3" t="s">
@@ -980,7 +979,7 @@
       <c r="P7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="X7" s="1" t="s">
+      <c r="X7" s="3" t="s">
         <v>13</v>
       </c>
       <c r="AA7" s="3" t="s">
@@ -1079,7 +1078,7 @@
       </c>
     </row>
     <row r="10" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="2" t="s">
         <v>7</v>
       </c>
       <c r="G10" s="3" t="s">
@@ -1094,13 +1093,13 @@
       <c r="W10" t="s">
         <v>13</v>
       </c>
-      <c r="X10" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y10" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z10" s="1" t="s">
+      <c r="X10" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y10" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z10" s="3" t="s">
         <v>13</v>
       </c>
       <c r="AA10" s="3" t="s">
@@ -1111,7 +1110,7 @@
       </c>
     </row>
     <row r="11" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
       <c r="I11" t="s">
@@ -1150,13 +1149,13 @@
       <c r="W11" t="s">
         <v>13</v>
       </c>
-      <c r="X11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z11" s="1" t="s">
+      <c r="X11" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y11" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z11" s="3" t="s">
         <v>13</v>
       </c>
       <c r="AA11" s="3" t="s">
@@ -1199,7 +1198,7 @@
       <c r="T13" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="Z13" s="1" t="s">
+      <c r="Z13" s="3" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1215,13 +1214,13 @@
       </c>
     </row>
     <row r="15" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="A15" s="2" t="s">
         <v>11</v>
       </c>
       <c r="W15" t="s">
         <v>13</v>
       </c>
-      <c r="X15" s="1" t="s">
+      <c r="X15" s="3" t="s">
         <v>13</v>
       </c>
       <c r="AA15" s="3" t="s">

</xml_diff>